<commit_message>
Clouds now go back to 1999
</commit_message>
<xml_diff>
--- a/data/HistSLOAD.xlsx
+++ b/data/HistSLOAD.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfelletter\Documents\RW-RDF-Process-Plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2AAD6E-6B8E-4D36-9D19-5FCEF19CDB4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438054DF-856B-43B4-A1B9-AF4418F2FE46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10440" windowHeight="5520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="HistSLOAD" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="7">
   <si>
     <t>Year</t>
   </si>
@@ -193,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +371,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -534,8 +540,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -622,23 +629,78 @@
       <sheetName val="Fig 20 IMPER"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
       <sheetData sheetId="16">
+        <row r="62">
+          <cell r="B62">
+            <v>420</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="B63">
+            <v>439</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="B64">
+            <v>452</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="B65">
+            <v>471</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="B66">
+            <v>511</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="B67">
+            <v>526</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="B68">
+            <v>505</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="B69">
+            <v>472</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="B70">
+            <v>475</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="B71">
+            <v>464</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="B72">
+            <v>423</v>
+          </cell>
+        </row>
         <row r="73">
           <cell r="B73">
             <v>431</v>
@@ -685,9 +747,64 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
       <sheetData sheetId="19">
+        <row r="62">
+          <cell r="B62">
+            <v>549</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="B63">
+            <v>539</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="B64">
+            <v>550</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="B65">
+            <v>561</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="B66">
+            <v>584</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="B67">
+            <v>625</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="B68">
+            <v>643</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="B69">
+            <v>646</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="B70">
+            <v>632</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="B71">
+            <v>620</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="B72">
+            <v>604</v>
+          </cell>
+        </row>
         <row r="73">
           <cell r="B73">
             <v>577</v>
@@ -735,6 +852,61 @@
         </row>
       </sheetData>
       <sheetData sheetId="20">
+        <row r="62">
+          <cell r="B62">
+            <v>550</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="B63">
+            <v>549</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="B64">
+            <v>549</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="B65">
+            <v>572</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="B66">
+            <v>592</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="B67">
+            <v>644</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="B68">
+            <v>668</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="B69">
+            <v>671</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="B70">
+            <v>657</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="B71">
+            <v>644</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="B72">
+            <v>624</v>
+          </cell>
+        </row>
         <row r="73">
           <cell r="B73">
             <v>600</v>
@@ -782,6 +954,61 @@
         </row>
       </sheetData>
       <sheetData sheetId="21">
+        <row r="62">
+          <cell r="B62">
+            <v>670</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="B63">
+            <v>661</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="B64">
+            <v>680</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="B65">
+            <v>689</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="B66">
+            <v>695</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="B67">
+            <v>729</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="B68">
+            <v>710</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="B69">
+            <v>720</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="B70">
+            <v>715</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="B71">
+            <v>733</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="B72">
+            <v>717</v>
+          </cell>
+        </row>
         <row r="73">
           <cell r="B73">
             <v>690</v>
@@ -1129,11 +1356,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FA3F15-F84C-4733-AC4D-279958C970B8}">
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+      <selection activeCell="B62" sqref="B62:C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,434 +1377,962 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B2">
+        <f>'[1]Fig 15 LEES'!$B62</f>
+        <v>420</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2000</v>
+      </c>
+      <c r="B3">
+        <f>'[1]Fig 15 LEES'!$B63</f>
+        <v>439</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2001</v>
+      </c>
+      <c r="B4">
+        <f>'[1]Fig 15 LEES'!$B64</f>
+        <v>452</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2002</v>
+      </c>
+      <c r="B5">
+        <f>'[1]Fig 15 LEES'!$B65</f>
+        <v>471</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2003</v>
+      </c>
+      <c r="B6">
+        <f>'[1]Fig 15 LEES'!$B66</f>
+        <v>511</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2004</v>
+      </c>
+      <c r="B7">
+        <f>'[1]Fig 15 LEES'!$B67</f>
+        <v>526</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2005</v>
+      </c>
+      <c r="B8">
+        <f>'[1]Fig 15 LEES'!$B68</f>
+        <v>505</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2006</v>
+      </c>
+      <c r="B9">
+        <f>'[1]Fig 15 LEES'!$B69</f>
+        <v>472</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2007</v>
+      </c>
+      <c r="B10">
+        <f>'[1]Fig 15 LEES'!$B70</f>
+        <v>475</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2008</v>
+      </c>
+      <c r="B11">
+        <f>'[1]Fig 15 LEES'!$B71</f>
+        <v>464</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2009</v>
+      </c>
+      <c r="B12">
+        <f>'[1]Fig 15 LEES'!$B72</f>
+        <v>423</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2010</v>
       </c>
-      <c r="B2">
+      <c r="B13">
         <f>'[1]Fig 15 LEES'!$B73</f>
         <v>431</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>2011</v>
       </c>
-      <c r="B3">
+      <c r="B14">
         <f>'[1]Fig 15 LEES'!$B74</f>
         <v>435</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>2012</v>
       </c>
-      <c r="B4">
+      <c r="B15">
         <f>'[1]Fig 15 LEES'!$B75</f>
         <v>420</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>2013</v>
       </c>
-      <c r="B5">
+      <c r="B16">
         <f>'[1]Fig 15 LEES'!$B76</f>
         <v>473</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>2014</v>
       </c>
-      <c r="B6">
+      <c r="B17">
         <f>'[1]Fig 15 LEES'!$B77</f>
         <v>525</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>2015</v>
       </c>
-      <c r="B7">
+      <c r="B18">
         <f>'[1]Fig 15 LEES'!$B78</f>
         <v>468</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>2016</v>
       </c>
-      <c r="B8">
+      <c r="B19">
         <f>'[1]Fig 15 LEES'!$B79</f>
         <v>468</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>2017</v>
       </c>
-      <c r="B9">
+      <c r="B20">
         <f>'[1]Fig 15 LEES'!$B80</f>
         <v>460</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>2018</v>
       </c>
-      <c r="B10">
+      <c r="B21">
         <f>'[1]Fig 15 LEES'!$B81</f>
         <v>413</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B22">
+        <f>'[1]Fig 18 HOOVER'!$B62</f>
+        <v>549</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2000</v>
+      </c>
+      <c r="B23">
+        <f>'[1]Fig 18 HOOVER'!$B63</f>
+        <v>539</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2001</v>
+      </c>
+      <c r="B24">
+        <f>'[1]Fig 18 HOOVER'!$B64</f>
+        <v>550</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2002</v>
+      </c>
+      <c r="B25">
+        <f>'[1]Fig 18 HOOVER'!$B65</f>
+        <v>561</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2003</v>
+      </c>
+      <c r="B26">
+        <f>'[1]Fig 18 HOOVER'!$B66</f>
+        <v>584</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2004</v>
+      </c>
+      <c r="B27">
+        <f>'[1]Fig 18 HOOVER'!$B67</f>
+        <v>625</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2005</v>
+      </c>
+      <c r="B28">
+        <f>'[1]Fig 18 HOOVER'!$B68</f>
+        <v>643</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2006</v>
+      </c>
+      <c r="B29">
+        <f>'[1]Fig 18 HOOVER'!$B69</f>
+        <v>646</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2007</v>
+      </c>
+      <c r="B30">
+        <f>'[1]Fig 18 HOOVER'!$B70</f>
+        <v>632</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2008</v>
+      </c>
+      <c r="B31">
+        <f>'[1]Fig 18 HOOVER'!$B71</f>
+        <v>620</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2009</v>
+      </c>
+      <c r="B32">
+        <f>'[1]Fig 18 HOOVER'!$B72</f>
+        <v>604</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>2010</v>
       </c>
-      <c r="B11">
+      <c r="B33">
         <f>'[1]Fig 18 HOOVER'!$B73</f>
         <v>577</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C33" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>2011</v>
       </c>
-      <c r="B12">
+      <c r="B34">
         <f>'[1]Fig 18 HOOVER'!$B74</f>
         <v>568</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>2012</v>
       </c>
-      <c r="B13">
+      <c r="B35">
         <f>'[1]Fig 18 HOOVER'!$B75</f>
         <v>548</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>2013</v>
       </c>
-      <c r="B14">
+      <c r="B36">
         <f>'[1]Fig 18 HOOVER'!$B76</f>
         <v>551</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C36" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>2014</v>
       </c>
-      <c r="B15">
+      <c r="B37">
         <f>'[1]Fig 18 HOOVER'!$B77</f>
         <v>575</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>2015</v>
       </c>
-      <c r="B16">
+      <c r="B38">
         <f>'[1]Fig 18 HOOVER'!$B78</f>
         <v>614</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C38" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>2016</v>
       </c>
-      <c r="B17">
+      <c r="B39">
         <f>'[1]Fig 18 HOOVER'!$B79</f>
         <v>598</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>2017</v>
       </c>
-      <c r="B18">
+      <c r="B40">
         <f>'[1]Fig 18 HOOVER'!$B80</f>
         <v>596</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C40" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>2018</v>
       </c>
-      <c r="B19">
+      <c r="B41">
         <f>'[1]Fig 18 HOOVER'!$B81</f>
         <v>574</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C41" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B42">
+        <f>'[1]Fig 19 PARKER'!$B62</f>
+        <v>550</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2000</v>
+      </c>
+      <c r="B43">
+        <f>'[1]Fig 19 PARKER'!$B63</f>
+        <v>549</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2001</v>
+      </c>
+      <c r="B44">
+        <f>'[1]Fig 19 PARKER'!$B64</f>
+        <v>549</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2002</v>
+      </c>
+      <c r="B45">
+        <f>'[1]Fig 19 PARKER'!$B65</f>
+        <v>572</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2003</v>
+      </c>
+      <c r="B46">
+        <f>'[1]Fig 19 PARKER'!$B66</f>
+        <v>592</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2004</v>
+      </c>
+      <c r="B47">
+        <f>'[1]Fig 19 PARKER'!$B67</f>
+        <v>644</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2005</v>
+      </c>
+      <c r="B48">
+        <f>'[1]Fig 19 PARKER'!$B68</f>
+        <v>668</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2006</v>
+      </c>
+      <c r="B49">
+        <f>'[1]Fig 19 PARKER'!$B69</f>
+        <v>671</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2007</v>
+      </c>
+      <c r="B50">
+        <f>'[1]Fig 19 PARKER'!$B70</f>
+        <v>657</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2008</v>
+      </c>
+      <c r="B51">
+        <f>'[1]Fig 19 PARKER'!$B71</f>
+        <v>644</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2009</v>
+      </c>
+      <c r="B52">
+        <f>'[1]Fig 19 PARKER'!$B72</f>
+        <v>624</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>2010</v>
       </c>
-      <c r="B20">
+      <c r="B53">
         <f>'[1]Fig 19 PARKER'!$B73</f>
         <v>600</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C53" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>2011</v>
       </c>
-      <c r="B21">
+      <c r="B54">
         <f>'[1]Fig 19 PARKER'!$B74</f>
         <v>591</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C54" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>2012</v>
       </c>
-      <c r="B22">
+      <c r="B55">
         <f>'[1]Fig 19 PARKER'!$B75</f>
         <v>569</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C55" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>2013</v>
       </c>
-      <c r="B23">
+      <c r="B56">
         <f>'[1]Fig 19 PARKER'!$B76</f>
         <v>567</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C56" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>2014</v>
       </c>
-      <c r="B24">
+      <c r="B57">
         <f>'[1]Fig 19 PARKER'!$B77</f>
         <v>595</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C57" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>2015</v>
       </c>
-      <c r="B25">
+      <c r="B58">
         <f>'[1]Fig 19 PARKER'!$B78</f>
         <v>634</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>2016</v>
       </c>
-      <c r="B26">
+      <c r="B59">
         <f>'[1]Fig 19 PARKER'!$B79</f>
         <v>624</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C59" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>2017</v>
       </c>
-      <c r="B27">
+      <c r="B60">
         <f>'[1]Fig 19 PARKER'!$B80</f>
         <v>615</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>2018</v>
       </c>
-      <c r="B28">
+      <c r="B61">
         <f>'[1]Fig 19 PARKER'!$B81</f>
         <v>591</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C61" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B62">
+        <f>'[1]Fig 20 IMPER'!$B62</f>
+        <v>670</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2000</v>
+      </c>
+      <c r="B63">
+        <f>'[1]Fig 20 IMPER'!$B63</f>
+        <v>661</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2001</v>
+      </c>
+      <c r="B64">
+        <f>'[1]Fig 20 IMPER'!$B64</f>
+        <v>680</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2002</v>
+      </c>
+      <c r="B65">
+        <f>'[1]Fig 20 IMPER'!$B65</f>
+        <v>689</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2003</v>
+      </c>
+      <c r="B66">
+        <f>'[1]Fig 20 IMPER'!$B66</f>
+        <v>695</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2004</v>
+      </c>
+      <c r="B67">
+        <f>'[1]Fig 20 IMPER'!$B67</f>
+        <v>729</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2005</v>
+      </c>
+      <c r="B68">
+        <f>'[1]Fig 20 IMPER'!$B68</f>
+        <v>710</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2006</v>
+      </c>
+      <c r="B69">
+        <f>'[1]Fig 20 IMPER'!$B69</f>
+        <v>720</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2007</v>
+      </c>
+      <c r="B70">
+        <f>'[1]Fig 20 IMPER'!$B70</f>
+        <v>715</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2008</v>
+      </c>
+      <c r="B71">
+        <f>'[1]Fig 20 IMPER'!$B71</f>
+        <v>733</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2009</v>
+      </c>
+      <c r="B72">
+        <f>'[1]Fig 20 IMPER'!$B72</f>
+        <v>717</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>2010</v>
       </c>
-      <c r="B29">
+      <c r="B73">
         <f>'[1]Fig 20 IMPER'!$B73</f>
         <v>690</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C73" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>2011</v>
       </c>
-      <c r="B30">
+      <c r="B74">
         <f>'[1]Fig 20 IMPER'!$B74</f>
         <v>681</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C74" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>2012</v>
       </c>
-      <c r="B31">
+      <c r="B75">
         <f>'[1]Fig 20 IMPER'!$B75</f>
         <v>677</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C75" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>2013</v>
       </c>
-      <c r="B32">
+      <c r="B76">
         <f>'[1]Fig 20 IMPER'!$B76</f>
         <v>677</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C76" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>2014</v>
       </c>
-      <c r="B33">
+      <c r="B77">
         <f>'[1]Fig 20 IMPER'!$B77</f>
         <v>697</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C77" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>2015</v>
       </c>
-      <c r="B34">
+      <c r="B78">
         <f>'[1]Fig 20 IMPER'!$B78</f>
         <v>726</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C78" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>2016</v>
       </c>
-      <c r="B35">
+      <c r="B79">
         <f>'[1]Fig 20 IMPER'!$B79</f>
         <v>715</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C79" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>2017</v>
       </c>
-      <c r="B36">
+      <c r="B80">
         <f>'[1]Fig 20 IMPER'!$B80</f>
         <v>703</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C80" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
         <v>2018</v>
       </c>
-      <c r="B37">
+      <c r="B81">
         <f>'[1]Fig 20 IMPER'!$B81</f>
         <v>683</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C81" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Scripts for June 23 Forum Mtg
Update HistSLOAD to include 2022 values for plots
</commit_message>
<xml_diff>
--- a/data/HistSLOAD.xlsx
+++ b/data/HistSLOAD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfelletter\Documents\RW-RDF-Process-Plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310C1634-8817-4E29-9EF6-3183BDBADF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2011261F-AA8F-4C1C-A346-D986A94B58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11610" yWindow="1005" windowWidth="16200" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>tc={B6E8A236-6550-495D-8B00-1B076CB93976}</author>
   </authors>
   <commentList>
-    <comment ref="B94" authorId="0" shapeId="0" xr:uid="{B6E8A236-6550-495D-8B00-1B076CB93976}">
+    <comment ref="B98" authorId="0" shapeId="0" xr:uid="{B6E8A236-6550-495D-8B00-1B076CB93976}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="8">
   <si>
     <t>Year</t>
   </si>
@@ -82,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,12 +216,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -992,6 +986,20 @@
           </cell>
           <cell r="AA101">
             <v>646.84095907123367</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="V102">
+            <v>512.91634697834195</v>
+          </cell>
+          <cell r="Y102">
+            <v>565.57815637515068</v>
+          </cell>
+          <cell r="Z102">
+            <v>574.54588838315988</v>
+          </cell>
+          <cell r="AA102">
+            <v>670.99508532151037</v>
           </cell>
         </row>
       </sheetData>
@@ -1304,7 +1312,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B94" dT="2022-08-24T17:17:55.15" personId="{251DFD64-29ED-494F-8A67-0844219D385F}" id="{B6E8A236-6550-495D-8B00-1B076CB93976}">
+  <threadedComment ref="B98" dT="2022-08-24T17:17:55.15" personId="{251DFD64-29ED-494F-8A67-0844219D385F}" id="{B6E8A236-6550-495D-8B00-1B076CB93976}">
     <text>Taken from 2020 NFS model Annual Natural Salt.PwllInflw_FWAAC</text>
   </threadedComment>
 </ThreadedComments>
@@ -1312,15 +1320,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FA3F15-F84C-4733-AC4D-279958C970B8}">
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1999</v>
       </c>
@@ -1343,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -1355,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2001</v>
       </c>
@@ -1367,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2002</v>
       </c>
@@ -1379,7 +1387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2003</v>
       </c>
@@ -1391,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2004</v>
       </c>
@@ -1403,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2005</v>
       </c>
@@ -1415,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2006</v>
       </c>
@@ -1427,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2007</v>
       </c>
@@ -1439,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2008</v>
       </c>
@@ -1451,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -1463,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2010</v>
       </c>
@@ -1475,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -1487,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2012</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2013</v>
       </c>
@@ -1511,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2014</v>
       </c>
@@ -1523,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2015</v>
       </c>
@@ -1535,7 +1543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -1547,7 +1555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2017</v>
       </c>
@@ -1559,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2018</v>
       </c>
@@ -1571,7 +1579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1583,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -1595,7 +1603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -1607,1073 +1615,1121 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2022</v>
+      </c>
+      <c r="B25" s="2">
+        <f>ROUND([1]annualCYConc!$V102,0)</f>
+        <v>513</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
         <v>1999</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="2">
         <f>ROUND([1]annualCYConc!$Y79,0)</f>
         <v>549</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>2000</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="2">
         <f>ROUND([1]annualCYConc!$Y80,0)</f>
         <v>541</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>2001</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B28" s="2">
         <f>ROUND([1]annualCYConc!$Y81,0)</f>
         <v>550</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>2002</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="2">
         <f>ROUND([1]annualCYConc!$Y82,0)</f>
         <v>564</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>2003</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B30" s="2">
         <f>ROUND([1]annualCYConc!$Y83,0)</f>
         <v>584</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>2004</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="2">
         <f>ROUND([1]annualCYConc!$Y84,0)</f>
         <v>623</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>2005</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="2">
         <f>ROUND([1]annualCYConc!$Y85,0)</f>
         <v>643</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
         <v>2006</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="2">
         <f>ROUND([1]annualCYConc!$Y86,0)</f>
         <v>647</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>2007</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="2">
         <f>ROUND([1]annualCYConc!$Y87,0)</f>
         <v>632</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
         <v>2008</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B35" s="2">
         <f>ROUND([1]annualCYConc!$Y88,0)</f>
         <v>622</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>2009</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B36" s="2">
         <f>ROUND([1]annualCYConc!$Y89,0)</f>
         <v>604</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>2010</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B37" s="2">
         <f>ROUND([1]annualCYConc!$Y90,0)</f>
         <v>576</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
         <v>2011</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B38" s="2">
         <f>ROUND([1]annualCYConc!$Y91,0)</f>
         <v>568</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
         <v>2012</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B39" s="2">
         <f>ROUND([1]annualCYConc!$Y92,0)</f>
         <v>548</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
         <v>2013</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B40" s="2">
         <f>ROUND([1]annualCYConc!$Y93,0)</f>
         <v>551</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>2014</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B41" s="2">
         <f>ROUND([1]annualCYConc!$Y94,0)</f>
         <v>581</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
         <v>2015</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B42" s="2">
         <f>ROUND([1]annualCYConc!$Y95,0)</f>
         <v>614</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
         <v>2016</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B43" s="2">
         <f>ROUND([1]annualCYConc!$Y96,0)</f>
         <v>598</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
         <v>2017</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B44" s="2">
         <f>ROUND([1]annualCYConc!$Y97,0)</f>
         <v>595</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
         <v>2018</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B45" s="2">
         <f>ROUND([1]annualCYConc!$Y98,0)</f>
         <v>571</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
         <v>2019</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B46" s="2">
         <f>ROUND([1]annualCYConc!$Y99,0)</f>
         <v>559</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
         <v>2020</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B47" s="2">
         <f>ROUND([1]annualCYConc!$Y100,0)</f>
         <v>560</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
         <v>2021</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B48" s="2">
         <f>ROUND([1]annualCYConc!$Y101,0)</f>
         <v>558</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2022</v>
+      </c>
+      <c r="B49" s="2">
+        <f>ROUND([1]annualCYConc!$Y102,0)</f>
+        <v>566</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
         <v>1999</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B50" s="2">
         <f>ROUND([1]annualCYConc!$Z79,0)</f>
         <v>550</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
         <v>2000</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B51" s="2">
         <f>ROUND([1]annualCYConc!$Z80,0)</f>
         <v>545</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C51" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
         <v>2001</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B52" s="2">
         <f>ROUND([1]annualCYConc!$Z81,0)</f>
         <v>549</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
         <v>2002</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B53" s="2">
         <f>ROUND([1]annualCYConc!$Z82,0)</f>
         <v>569</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
         <v>2003</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B54" s="2">
         <f>ROUND([1]annualCYConc!$Z83,0)</f>
         <v>592</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
         <v>2004</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B55" s="2">
         <f>ROUND([1]annualCYConc!$Z84,0)</f>
         <v>621</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
         <v>2005</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B56" s="2">
         <f>ROUND([1]annualCYConc!$Z85,0)</f>
         <v>668</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
         <v>2006</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B57" s="2">
         <f>ROUND([1]annualCYConc!$Z86,0)</f>
         <v>673</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
         <v>2007</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B58" s="2">
         <f>ROUND([1]annualCYConc!$Z87,0)</f>
         <v>657</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
         <v>2008</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B59" s="2">
         <f>ROUND([1]annualCYConc!$Z88,0)</f>
         <v>646</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
         <v>2009</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B60" s="2">
         <f>ROUND([1]annualCYConc!$Z89,0)</f>
         <v>624</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
         <v>2010</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B61" s="2">
         <f>ROUND([1]annualCYConc!$Z90,0)</f>
         <v>596</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C61" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
         <v>2011</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B62" s="2">
         <f>ROUND([1]annualCYConc!$Z91,0)</f>
         <v>591</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C62" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
         <v>2012</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B63" s="2">
         <f>ROUND([1]annualCYConc!$Z92,0)</f>
         <v>571</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
         <v>2013</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B64" s="2">
         <f>ROUND([1]annualCYConc!$Z93,0)</f>
         <v>567</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
         <v>2014</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B65" s="2">
         <f>ROUND([1]annualCYConc!$Z94,0)</f>
         <v>598</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C65" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
         <v>2015</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B66" s="2">
         <f>ROUND([1]annualCYConc!$Z95,0)</f>
         <v>634</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
         <v>2016</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B67" s="2">
         <f>ROUND([1]annualCYConc!$Z96,0)</f>
         <v>624</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C67" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
         <v>2017</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B68" s="2">
         <f>ROUND([1]annualCYConc!$Z97,0)</f>
         <v>615</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69">
         <v>2018</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B69" s="2">
         <f>ROUND([1]annualCYConc!$Z98,0)</f>
         <v>592</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70">
         <v>2019</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B70" s="2">
         <f>ROUND([1]annualCYConc!$Z99,0)</f>
         <v>575</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C70" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71">
         <v>2020</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B71" s="2">
         <f>ROUND([1]annualCYConc!$Z100,0)</f>
         <v>576</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C71" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
         <v>2021</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B72" s="2">
         <f>ROUND([1]annualCYConc!$Z101,0)</f>
         <v>572</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>2022</v>
+      </c>
+      <c r="B73" s="2">
+        <f>ROUND([1]annualCYConc!$Z102,0)</f>
+        <v>575</v>
+      </c>
+      <c r="C73" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
         <v>1999</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B74" s="2">
         <f>ROUND([1]annualCYConc!$AA79,0)</f>
         <v>670</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C74" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75">
         <v>2000</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B75" s="2">
         <f>ROUND([1]annualCYConc!$AA80,0)</f>
         <v>671</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C75" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76">
         <v>2001</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B76" s="2">
         <f>ROUND([1]annualCYConc!$AA81,0)</f>
         <v>680</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C76" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77">
         <v>2002</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B77" s="2">
         <f>ROUND([1]annualCYConc!$AA82,0)</f>
         <v>690</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C77" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78">
         <v>2003</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B78" s="2">
         <f>ROUND([1]annualCYConc!$AA83,0)</f>
         <v>695</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C78" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79">
         <v>2004</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B79" s="2">
         <f>ROUND([1]annualCYConc!$AA84,0)</f>
         <v>727</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C79" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80">
         <v>2005</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B80" s="2">
         <f>ROUND([1]annualCYConc!$AA85,0)</f>
         <v>710</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C80" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81">
         <v>2006</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B81" s="2">
         <f>ROUND([1]annualCYConc!$AA86,0)</f>
         <v>712</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C81" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82">
         <v>2007</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B82" s="2">
         <f>ROUND([1]annualCYConc!$AA87,0)</f>
         <v>715</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C82" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83">
         <v>2008</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B83" s="2">
         <f>ROUND([1]annualCYConc!$AA88,0)</f>
         <v>717</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C83" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84">
         <v>2009</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B84" s="2">
         <f>ROUND([1]annualCYConc!$AA89,0)</f>
         <v>717</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C84" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85">
         <v>2010</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B85" s="2">
         <f>ROUND([1]annualCYConc!$AA90,0)</f>
         <v>690</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C85" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86">
         <v>2011</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B86" s="2">
         <f>ROUND([1]annualCYConc!$AA91,0)</f>
         <v>681</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C86" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87">
         <v>2012</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B87" s="2">
         <f>ROUND([1]annualCYConc!$AA92,0)</f>
         <v>676</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C87" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88">
         <v>2013</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B88" s="2">
         <f>ROUND([1]annualCYConc!$AA93,0)</f>
         <v>677</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C88" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89">
         <v>2014</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B89" s="2">
         <f>ROUND([1]annualCYConc!$AA94,0)</f>
         <v>695</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C89" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90">
         <v>2015</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B90" s="2">
         <f>ROUND([1]annualCYConc!$AA95,0)</f>
         <v>726</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C90" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91">
         <v>2016</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B91" s="2">
         <f>ROUND([1]annualCYConc!$AA96,0)</f>
         <v>715</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C91" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92">
         <v>2017</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B92" s="2">
         <f>ROUND([1]annualCYConc!$AA97,0)</f>
         <v>702</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C92" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93">
         <v>2018</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B93" s="2">
         <f>ROUND([1]annualCYConc!$AA98,0)</f>
         <v>677</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C93" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94">
         <v>2019</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B94" s="2">
         <f>ROUND([1]annualCYConc!$AA99,0)</f>
         <v>655</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C94" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95">
         <v>2020</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B95" s="2">
         <f>ROUND([1]annualCYConc!$AA100,0)</f>
         <v>660</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C95" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96">
         <v>2021</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B96" s="2">
         <f>ROUND([1]annualCYConc!$AA101,0)</f>
         <v>647</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>2022</v>
+      </c>
+      <c r="B97" s="2">
+        <f>ROUND([1]annualCYConc!$AA102,0)</f>
+        <v>671</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="1">
         <v>1999</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B98" s="3">
         <v>424.38</v>
-      </c>
-      <c r="C94" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>2000</v>
-      </c>
-      <c r="B95" s="3">
-        <v>466.02</v>
-      </c>
-      <c r="C95" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>2001</v>
-      </c>
-      <c r="B96" s="3">
-        <v>472.19</v>
-      </c>
-      <c r="C96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>2002</v>
-      </c>
-      <c r="B97" s="3">
-        <v>500.17</v>
-      </c>
-      <c r="C97" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>2003</v>
-      </c>
-      <c r="B98" s="3">
-        <v>582.27</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>2004</v>
+        <v>2000</v>
       </c>
       <c r="B99" s="3">
-        <v>506.77</v>
+        <v>466.02</v>
       </c>
       <c r="C99" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>2005</v>
+        <v>2001</v>
       </c>
       <c r="B100" s="3">
-        <v>434.01</v>
+        <v>472.19</v>
       </c>
       <c r="C100" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>2006</v>
+        <v>2002</v>
       </c>
       <c r="B101" s="3">
-        <v>448.78</v>
+        <v>500.17</v>
       </c>
       <c r="C101" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="B102" s="3">
-        <v>487.3</v>
+        <v>582.27</v>
       </c>
       <c r="C102" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>2008</v>
+        <v>2004</v>
       </c>
       <c r="B103" s="3">
-        <v>396.75</v>
+        <v>506.77</v>
       </c>
       <c r="C103" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="B104" s="3">
-        <v>347.55</v>
+        <v>434.01</v>
       </c>
       <c r="C104" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="B105" s="3">
-        <v>487.06</v>
+        <v>448.78</v>
       </c>
       <c r="C105" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="B106" s="3">
-        <v>342.37</v>
+        <v>487.3</v>
       </c>
       <c r="C106" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="B107" s="3">
-        <v>590.34</v>
+        <v>396.75</v>
       </c>
       <c r="C107" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>2013</v>
+        <v>2009</v>
       </c>
       <c r="B108" s="3">
-        <v>607.6</v>
+        <v>347.55</v>
       </c>
       <c r="C108" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="B109" s="3">
-        <v>499.92</v>
+        <v>487.06</v>
       </c>
       <c r="C109" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="B110" s="3">
-        <v>404.57</v>
+        <v>342.37</v>
       </c>
       <c r="C110" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="B111" s="3">
-        <v>439.85</v>
+        <v>590.34</v>
       </c>
       <c r="C111" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="B112" s="3">
-        <v>437.95</v>
+        <v>607.6</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="B113" s="3">
-        <v>428.79</v>
+        <v>499.92</v>
       </c>
       <c r="C113" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="B114" s="3">
-        <v>401.49</v>
+        <v>404.57</v>
       </c>
       <c r="C114" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
+        <v>2016</v>
+      </c>
+      <c r="B115" s="3">
+        <v>439.85</v>
+      </c>
+      <c r="C115" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>2017</v>
+      </c>
+      <c r="B116" s="3">
+        <v>437.95</v>
+      </c>
+      <c r="C116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>2018</v>
+      </c>
+      <c r="B117" s="3">
+        <v>428.79</v>
+      </c>
+      <c r="C117" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>2019</v>
+      </c>
+      <c r="B118" s="3">
+        <v>401.49</v>
+      </c>
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119">
         <v>2020</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B119" s="3">
         <v>450.56</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C119" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New plots of UB trib concentrations Custom_WQAnn_CloudswHist.R
New script to plot GainsSaltMass_InputPlots.R
</commit_message>
<xml_diff>
--- a/data/HistSLOAD.xlsx
+++ b/data/HistSLOAD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfelletter\Documents\RW-RDF-Process-Plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2011261F-AA8F-4C1C-A346-D986A94B58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04874CCD-554B-4942-91E4-3181CA9999C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33120" yWindow="3030" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="11">
   <si>
     <t>Year</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>AnnlSlntyPwllInflw_FWAAC</t>
+  </si>
+  <si>
+    <t>Bluff_FWAAC</t>
+  </si>
+  <si>
+    <t>GreenRiverUTGreen_FWAAC</t>
+  </si>
+  <si>
+    <t>CiscoColorado_FWAAC</t>
   </si>
 </sst>
 </file>
@@ -629,8 +638,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Instructions"/>
       <sheetName val="ConcFlowLoad Figures"/>
@@ -645,6 +657,7 @@
       <sheetName val="Compare_RWInput"/>
       <sheetName val="monthlySaltMass"/>
       <sheetName val="annualCYFlow"/>
+      <sheetName val="compareParkerAnnual"/>
       <sheetName val="annualCYSaltMass"/>
       <sheetName val="annualCYConc"/>
       <sheetName val="FactSheet"/>
@@ -665,8 +678,18 @@
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
-      <sheetData sheetId="14">
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15">
         <row r="79">
+          <cell r="J79">
+            <v>495.6216249891022</v>
+          </cell>
+          <cell r="R79">
+            <v>392.77181829025585</v>
+          </cell>
+          <cell r="U79">
+            <v>280.41613725681447</v>
+          </cell>
           <cell r="V79">
             <v>420.45009713995051</v>
           </cell>
@@ -681,6 +704,15 @@
           </cell>
         </row>
         <row r="80">
+          <cell r="J80">
+            <v>557.12835724766512</v>
+          </cell>
+          <cell r="R80">
+            <v>405.17469447643998</v>
+          </cell>
+          <cell r="U80">
+            <v>388.33048586465787</v>
+          </cell>
           <cell r="V80">
             <v>435.65393896760042</v>
           </cell>
@@ -695,6 +727,15 @@
           </cell>
         </row>
         <row r="81">
+          <cell r="J81">
+            <v>621.95230461321501</v>
+          </cell>
+          <cell r="R81">
+            <v>394.92013599867738</v>
+          </cell>
+          <cell r="U81">
+            <v>324.6496463923296</v>
+          </cell>
           <cell r="V81">
             <v>451.66859752634576</v>
           </cell>
@@ -709,6 +750,15 @@
           </cell>
         </row>
         <row r="82">
+          <cell r="J82">
+            <v>852.47150595054688</v>
+          </cell>
+          <cell r="R82">
+            <v>478.18980112573939</v>
+          </cell>
+          <cell r="U82">
+            <v>495.87709491877865</v>
+          </cell>
           <cell r="V82">
             <v>468.30492383618434</v>
           </cell>
@@ -723,6 +773,15 @@
           </cell>
         </row>
         <row r="83">
+          <cell r="J83">
+            <v>610.98532373756075</v>
+          </cell>
+          <cell r="R83">
+            <v>368.6783218324656</v>
+          </cell>
+          <cell r="U83">
+            <v>525.43504943148002</v>
+          </cell>
           <cell r="V83">
             <v>510.84631285485153</v>
           </cell>
@@ -737,6 +796,15 @@
           </cell>
         </row>
         <row r="84">
+          <cell r="J84">
+            <v>654.90021211565625</v>
+          </cell>
+          <cell r="R84">
+            <v>403.71257425554387</v>
+          </cell>
+          <cell r="U84">
+            <v>409.89493691413202</v>
+          </cell>
           <cell r="V84">
             <v>525.59532399774253</v>
           </cell>
@@ -751,6 +819,15 @@
           </cell>
         </row>
         <row r="85">
+          <cell r="J85">
+            <v>415.69083045490117</v>
+          </cell>
+          <cell r="R85">
+            <v>360.86674300263758</v>
+          </cell>
+          <cell r="U85">
+            <v>331.51715195326727</v>
+          </cell>
           <cell r="V85">
             <v>505.48722442639593</v>
           </cell>
@@ -765,6 +842,15 @@
           </cell>
         </row>
         <row r="86">
+          <cell r="J86">
+            <v>486.5424686498456</v>
+          </cell>
+          <cell r="R86">
+            <v>368.53115089305538</v>
+          </cell>
+          <cell r="U86">
+            <v>348.38534803620689</v>
+          </cell>
           <cell r="V86">
             <v>472.49342172927004</v>
           </cell>
@@ -779,6 +865,15 @@
           </cell>
         </row>
         <row r="87">
+          <cell r="J87">
+            <v>533.3699012440519</v>
+          </cell>
+          <cell r="R87">
+            <v>390.71189691938389</v>
+          </cell>
+          <cell r="U87">
+            <v>303.69251204600391</v>
+          </cell>
           <cell r="V87">
             <v>474.85121804195273</v>
           </cell>
@@ -793,6 +888,15 @@
           </cell>
         </row>
         <row r="88">
+          <cell r="J88">
+            <v>384.20196606809378</v>
+          </cell>
+          <cell r="R88">
+            <v>351.4514281058282</v>
+          </cell>
+          <cell r="U88">
+            <v>249.15347752484735</v>
+          </cell>
           <cell r="V88">
             <v>462.97387320094322</v>
           </cell>
@@ -807,6 +911,15 @@
           </cell>
         </row>
         <row r="89">
+          <cell r="J89">
+            <v>425.8555581354716</v>
+          </cell>
+          <cell r="R89">
+            <v>300.61201217241802</v>
+          </cell>
+          <cell r="U89">
+            <v>327.33552031762076</v>
+          </cell>
           <cell r="V89">
             <v>422.51021026714079</v>
           </cell>
@@ -821,6 +934,15 @@
           </cell>
         </row>
         <row r="90">
+          <cell r="J90">
+            <v>512.47248680300868</v>
+          </cell>
+          <cell r="R90">
+            <v>363.18298432241477</v>
+          </cell>
+          <cell r="U90">
+            <v>425.20681273548126</v>
+          </cell>
           <cell r="V90">
             <v>423.9092177817422</v>
           </cell>
@@ -835,6 +957,15 @@
           </cell>
         </row>
         <row r="91">
+          <cell r="J91">
+            <v>345.78382785806906</v>
+          </cell>
+          <cell r="R91">
+            <v>277.67236328083686</v>
+          </cell>
+          <cell r="U91">
+            <v>352.82910571780423</v>
+          </cell>
           <cell r="V91">
             <v>434.80735544506371</v>
           </cell>
@@ -849,6 +980,15 @@
           </cell>
         </row>
         <row r="92">
+          <cell r="J92">
+            <v>721.81391806391616</v>
+          </cell>
+          <cell r="R92">
+            <v>398.17173146551488</v>
+          </cell>
+          <cell r="U92">
+            <v>358.20348648218624</v>
+          </cell>
           <cell r="V92">
             <v>419.29364715786767</v>
           </cell>
@@ -863,6 +1003,15 @@
           </cell>
         </row>
         <row r="93">
+          <cell r="J93">
+            <v>644.17088284662827</v>
+          </cell>
+          <cell r="R93">
+            <v>393.97778229521043</v>
+          </cell>
+          <cell r="U93">
+            <v>492.22647554732663</v>
+          </cell>
           <cell r="V93">
             <v>472.93484055840599</v>
           </cell>
@@ -877,6 +1026,15 @@
           </cell>
         </row>
         <row r="94">
+          <cell r="J94">
+            <v>427.3025576912512</v>
+          </cell>
+          <cell r="R94">
+            <v>340.14664090162159</v>
+          </cell>
+          <cell r="U94">
+            <v>387.6690040310603</v>
+          </cell>
           <cell r="V94">
             <v>524.17098756723374</v>
           </cell>
@@ -884,13 +1042,22 @@
             <v>580.5639085626899</v>
           </cell>
           <cell r="Z94">
-            <v>598.31538033036065</v>
+            <v>598.38663045401381</v>
           </cell>
           <cell r="AA94">
             <v>694.97391634452947</v>
           </cell>
         </row>
         <row r="95">
+          <cell r="J95">
+            <v>457.77024442730158</v>
+          </cell>
+          <cell r="R95">
+            <v>376.05514434396207</v>
+          </cell>
+          <cell r="U95">
+            <v>357.05842469976801</v>
+          </cell>
           <cell r="V95">
             <v>467.531861657798</v>
           </cell>
@@ -898,13 +1065,22 @@
             <v>614.46262656833392</v>
           </cell>
           <cell r="Z95">
-            <v>634.43779939780177</v>
+            <v>634.21258094022483</v>
           </cell>
           <cell r="AA95">
             <v>726.39837094676898</v>
           </cell>
         </row>
         <row r="96">
+          <cell r="J96">
+            <v>464.58861006074642</v>
+          </cell>
+          <cell r="R96">
+            <v>355.27549011915158</v>
+          </cell>
+          <cell r="U96">
+            <v>328.13328637322496</v>
+          </cell>
           <cell r="V96">
             <v>467.48830427258952</v>
           </cell>
@@ -912,13 +1088,22 @@
             <v>598.01152691473669</v>
           </cell>
           <cell r="Z96">
-            <v>624.48908190894372</v>
+            <v>624.52463644690977</v>
           </cell>
           <cell r="AA96">
             <v>714.58273355927281</v>
           </cell>
         </row>
         <row r="97">
+          <cell r="J97">
+            <v>432.32765668840426</v>
+          </cell>
+          <cell r="R97">
+            <v>309.09990294003558</v>
+          </cell>
+          <cell r="U97">
+            <v>300.67285519148618</v>
+          </cell>
           <cell r="V97">
             <v>459.50682257086191</v>
           </cell>
@@ -926,13 +1111,22 @@
             <v>594.91218389970004</v>
           </cell>
           <cell r="Z97">
-            <v>614.92929793877101</v>
+            <v>614.87857453659797</v>
           </cell>
           <cell r="AA97">
             <v>701.97873564980023</v>
           </cell>
         </row>
         <row r="98">
+          <cell r="J98">
+            <v>686.7350862390673</v>
+          </cell>
+          <cell r="R98">
+            <v>368.37522935213985</v>
+          </cell>
+          <cell r="U98">
+            <v>411.66724998517179</v>
+          </cell>
           <cell r="V98">
             <v>432.563404774221</v>
           </cell>
@@ -940,13 +1134,22 @@
             <v>570.74758473938095</v>
           </cell>
           <cell r="Z98">
-            <v>591.56682541349687</v>
+            <v>591.75277811450724</v>
           </cell>
           <cell r="AA98">
             <v>677.33721154829936</v>
           </cell>
         </row>
         <row r="99">
+          <cell r="J99">
+            <v>381.01959004682004</v>
+          </cell>
+          <cell r="R99">
+            <v>293.24294128291132</v>
+          </cell>
+          <cell r="U99">
+            <v>296.93303881084563</v>
+          </cell>
           <cell r="V99">
             <v>454.75095108770984</v>
           </cell>
@@ -954,13 +1157,22 @@
             <v>558.88238510144868</v>
           </cell>
           <cell r="Z99">
-            <v>575.03453504680147</v>
+            <v>575.10504777124424</v>
           </cell>
           <cell r="AA99">
             <v>654.8045088192398</v>
           </cell>
         </row>
         <row r="100">
+          <cell r="J100">
+            <v>605.13271763370165</v>
+          </cell>
+          <cell r="R100">
+            <v>330.48270511014505</v>
+          </cell>
+          <cell r="U100">
+            <v>355.28393070800604</v>
+          </cell>
           <cell r="V100">
             <v>424.52585089473257</v>
           </cell>
@@ -975,6 +1187,15 @@
           </cell>
         </row>
         <row r="101">
+          <cell r="J101">
+            <v>713.37297512992711</v>
+          </cell>
+          <cell r="R101">
+            <v>402.08256408292164</v>
+          </cell>
+          <cell r="U101">
+            <v>399.0792475604689</v>
+          </cell>
           <cell r="V101">
             <v>450.12755221796908</v>
           </cell>
@@ -982,28 +1203,37 @@
             <v>558.45305967844797</v>
           </cell>
           <cell r="Z101">
-            <v>571.65799967846306</v>
+            <v>574.01936254773068</v>
           </cell>
           <cell r="AA101">
             <v>646.84095907123367</v>
           </cell>
         </row>
         <row r="102">
+          <cell r="J102">
+            <v>602.27786518460141</v>
+          </cell>
+          <cell r="R102">
+            <v>348.63728272888568</v>
+          </cell>
+          <cell r="U102">
+            <v>397.74396313567934</v>
+          </cell>
           <cell r="V102">
-            <v>512.91634697834195</v>
+            <v>512.41619419565552</v>
           </cell>
           <cell r="Y102">
-            <v>565.57815637515068</v>
+            <v>577.62217758435918</v>
           </cell>
           <cell r="Z102">
-            <v>574.54588838315988</v>
+            <v>574.54588841431507</v>
           </cell>
           <cell r="AA102">
-            <v>670.99508532151037</v>
+            <v>670.33774162667407</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1320,15 +1550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FA3F15-F84C-4733-AC4D-279958C970B8}">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:C97"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168:C191"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1339,7 +1569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1999</v>
       </c>
@@ -1351,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -1363,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2001</v>
       </c>
@@ -1375,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2002</v>
       </c>
@@ -1387,7 +1617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2003</v>
       </c>
@@ -1399,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2004</v>
       </c>
@@ -1411,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2005</v>
       </c>
@@ -1423,7 +1653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2006</v>
       </c>
@@ -1435,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2007</v>
       </c>
@@ -1447,7 +1677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2008</v>
       </c>
@@ -1459,7 +1689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -1471,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2010</v>
       </c>
@@ -1483,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -1495,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2012</v>
       </c>
@@ -1507,7 +1737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2013</v>
       </c>
@@ -1519,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2014</v>
       </c>
@@ -1531,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2015</v>
       </c>
@@ -1543,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -1555,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2017</v>
       </c>
@@ -1567,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2018</v>
       </c>
@@ -1579,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1591,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -1603,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -1615,19 +1845,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2022</v>
       </c>
       <c r="B25" s="2">
         <f>ROUND([1]annualCYConc!$V102,0)</f>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1999</v>
       </c>
@@ -1639,7 +1869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2000</v>
       </c>
@@ -1651,7 +1881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2001</v>
       </c>
@@ -1663,7 +1893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2002</v>
       </c>
@@ -1675,7 +1905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2003</v>
       </c>
@@ -1687,7 +1917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2004</v>
       </c>
@@ -1699,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2005</v>
       </c>
@@ -1711,7 +1941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2006</v>
       </c>
@@ -1723,7 +1953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2007</v>
       </c>
@@ -1735,7 +1965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2008</v>
       </c>
@@ -1747,7 +1977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2009</v>
       </c>
@@ -1759,7 +1989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2010</v>
       </c>
@@ -1771,7 +2001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -1783,7 +2013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2012</v>
       </c>
@@ -1795,7 +2025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2013</v>
       </c>
@@ -1807,7 +2037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2014</v>
       </c>
@@ -1819,7 +2049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2015</v>
       </c>
@@ -1831,7 +2061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2016</v>
       </c>
@@ -1843,7 +2073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2017</v>
       </c>
@@ -1855,7 +2085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2018</v>
       </c>
@@ -1867,7 +2097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2019</v>
       </c>
@@ -1879,7 +2109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2020</v>
       </c>
@@ -1891,7 +2121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -1903,19 +2133,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2022</v>
       </c>
       <c r="B49" s="2">
         <f>ROUND([1]annualCYConc!$Y102,0)</f>
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1999</v>
       </c>
@@ -1927,7 +2157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2000</v>
       </c>
@@ -1939,7 +2169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2001</v>
       </c>
@@ -1951,7 +2181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2002</v>
       </c>
@@ -1963,7 +2193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2003</v>
       </c>
@@ -1975,7 +2205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2004</v>
       </c>
@@ -1987,7 +2217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2005</v>
       </c>
@@ -1999,7 +2229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2006</v>
       </c>
@@ -2011,7 +2241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2007</v>
       </c>
@@ -2023,7 +2253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2008</v>
       </c>
@@ -2035,7 +2265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2009</v>
       </c>
@@ -2047,7 +2277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2010</v>
       </c>
@@ -2059,7 +2289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2011</v>
       </c>
@@ -2071,7 +2301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2012</v>
       </c>
@@ -2083,7 +2313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2013</v>
       </c>
@@ -2095,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2014</v>
       </c>
@@ -2107,7 +2337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2015</v>
       </c>
@@ -2119,19 +2349,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2016</v>
       </c>
       <c r="B67" s="2">
         <f>ROUND([1]annualCYConc!$Z96,0)</f>
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C67" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2017</v>
       </c>
@@ -2143,7 +2373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2018</v>
       </c>
@@ -2155,7 +2385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2019</v>
       </c>
@@ -2167,7 +2397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2020</v>
       </c>
@@ -2179,19 +2409,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2021</v>
       </c>
       <c r="B72" s="2">
         <f>ROUND([1]annualCYConc!$Z101,0)</f>
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -2203,7 +2433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1999</v>
       </c>
@@ -2215,7 +2445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2000</v>
       </c>
@@ -2227,7 +2457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2001</v>
       </c>
@@ -2239,7 +2469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2002</v>
       </c>
@@ -2251,7 +2481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2003</v>
       </c>
@@ -2263,7 +2493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2004</v>
       </c>
@@ -2275,7 +2505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2005</v>
       </c>
@@ -2287,7 +2517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2006</v>
       </c>
@@ -2299,7 +2529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2007</v>
       </c>
@@ -2311,7 +2541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2008</v>
       </c>
@@ -2323,7 +2553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2009</v>
       </c>
@@ -2335,7 +2565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2010</v>
       </c>
@@ -2347,7 +2577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2011</v>
       </c>
@@ -2359,7 +2589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2012</v>
       </c>
@@ -2371,7 +2601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2013</v>
       </c>
@@ -2383,7 +2613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2014</v>
       </c>
@@ -2395,7 +2625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2015</v>
       </c>
@@ -2407,7 +2637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2016</v>
       </c>
@@ -2419,7 +2649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2017</v>
       </c>
@@ -2431,7 +2661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2018</v>
       </c>
@@ -2443,7 +2673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2019</v>
       </c>
@@ -2455,7 +2685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2020</v>
       </c>
@@ -2467,7 +2697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2021</v>
       </c>
@@ -2479,19 +2709,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2022</v>
       </c>
       <c r="B97" s="2">
         <f>ROUND([1]annualCYConc!$AA102,0)</f>
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C97" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>1999</v>
       </c>
@@ -2502,7 +2732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2000</v>
       </c>
@@ -2513,7 +2743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2001</v>
       </c>
@@ -2524,7 +2754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2002</v>
       </c>
@@ -2535,7 +2765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2003</v>
       </c>
@@ -2546,7 +2776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2004</v>
       </c>
@@ -2557,7 +2787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2005</v>
       </c>
@@ -2568,7 +2798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2006</v>
       </c>
@@ -2579,7 +2809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2007</v>
       </c>
@@ -2590,7 +2820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2008</v>
       </c>
@@ -2601,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2009</v>
       </c>
@@ -2612,7 +2842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2010</v>
       </c>
@@ -2623,7 +2853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2011</v>
       </c>
@@ -2634,7 +2864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2012</v>
       </c>
@@ -2645,7 +2875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2013</v>
       </c>
@@ -2656,7 +2886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2014</v>
       </c>
@@ -2667,7 +2897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2015</v>
       </c>
@@ -2678,7 +2908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2016</v>
       </c>
@@ -2689,7 +2919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2017</v>
       </c>
@@ -2700,7 +2930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2018</v>
       </c>
@@ -2711,7 +2941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2019</v>
       </c>
@@ -2722,7 +2952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2020</v>
       </c>
@@ -2731,6 +2961,870 @@
       </c>
       <c r="C119" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B120" s="2">
+        <f>ROUND([1]annualCYConc!$U79,0)</f>
+        <v>280</v>
+      </c>
+      <c r="C120" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>2000</v>
+      </c>
+      <c r="B121" s="2">
+        <f>ROUND([1]annualCYConc!$U80,0)</f>
+        <v>388</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>2001</v>
+      </c>
+      <c r="B122" s="2">
+        <f>ROUND([1]annualCYConc!$U81,0)</f>
+        <v>325</v>
+      </c>
+      <c r="C122" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>2002</v>
+      </c>
+      <c r="B123" s="2">
+        <f>ROUND([1]annualCYConc!$U82,0)</f>
+        <v>496</v>
+      </c>
+      <c r="C123" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>2003</v>
+      </c>
+      <c r="B124" s="2">
+        <f>ROUND([1]annualCYConc!$U83,0)</f>
+        <v>525</v>
+      </c>
+      <c r="C124" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>2004</v>
+      </c>
+      <c r="B125" s="2">
+        <f>ROUND([1]annualCYConc!$U84,0)</f>
+        <v>410</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>2005</v>
+      </c>
+      <c r="B126" s="2">
+        <f>ROUND([1]annualCYConc!$U85,0)</f>
+        <v>332</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>2006</v>
+      </c>
+      <c r="B127" s="2">
+        <f>ROUND([1]annualCYConc!$U86,0)</f>
+        <v>348</v>
+      </c>
+      <c r="C127" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>2007</v>
+      </c>
+      <c r="B128" s="2">
+        <f>ROUND([1]annualCYConc!$U87,0)</f>
+        <v>304</v>
+      </c>
+      <c r="C128" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>2008</v>
+      </c>
+      <c r="B129" s="2">
+        <f>ROUND([1]annualCYConc!$U88,0)</f>
+        <v>249</v>
+      </c>
+      <c r="C129" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>2009</v>
+      </c>
+      <c r="B130" s="2">
+        <f>ROUND([1]annualCYConc!$U89,0)</f>
+        <v>327</v>
+      </c>
+      <c r="C130" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>2010</v>
+      </c>
+      <c r="B131" s="2">
+        <f>ROUND([1]annualCYConc!$U90,0)</f>
+        <v>425</v>
+      </c>
+      <c r="C131" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>2011</v>
+      </c>
+      <c r="B132" s="2">
+        <f>ROUND([1]annualCYConc!$U91,0)</f>
+        <v>353</v>
+      </c>
+      <c r="C132" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>2012</v>
+      </c>
+      <c r="B133" s="2">
+        <f>ROUND([1]annualCYConc!$U92,0)</f>
+        <v>358</v>
+      </c>
+      <c r="C133" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>2013</v>
+      </c>
+      <c r="B134" s="2">
+        <f>ROUND([1]annualCYConc!$U93,0)</f>
+        <v>492</v>
+      </c>
+      <c r="C134" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>2014</v>
+      </c>
+      <c r="B135" s="2">
+        <f>ROUND([1]annualCYConc!$U94,0)</f>
+        <v>388</v>
+      </c>
+      <c r="C135" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>2015</v>
+      </c>
+      <c r="B136" s="2">
+        <f>ROUND([1]annualCYConc!$U95,0)</f>
+        <v>357</v>
+      </c>
+      <c r="C136" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>2016</v>
+      </c>
+      <c r="B137" s="2">
+        <f>ROUND([1]annualCYConc!$U96,0)</f>
+        <v>328</v>
+      </c>
+      <c r="C137" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>2017</v>
+      </c>
+      <c r="B138" s="2">
+        <f>ROUND([1]annualCYConc!$U97,0)</f>
+        <v>301</v>
+      </c>
+      <c r="C138" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>2018</v>
+      </c>
+      <c r="B139" s="2">
+        <f>ROUND([1]annualCYConc!$U98,0)</f>
+        <v>412</v>
+      </c>
+      <c r="C139" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>2019</v>
+      </c>
+      <c r="B140" s="2">
+        <f>ROUND([1]annualCYConc!$U99,0)</f>
+        <v>297</v>
+      </c>
+      <c r="C140" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>2020</v>
+      </c>
+      <c r="B141" s="2">
+        <f>ROUND([1]annualCYConc!$U100,0)</f>
+        <v>355</v>
+      </c>
+      <c r="C141" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>2021</v>
+      </c>
+      <c r="B142" s="2">
+        <f>ROUND([1]annualCYConc!$U101,0)</f>
+        <v>399</v>
+      </c>
+      <c r="C142" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>2022</v>
+      </c>
+      <c r="B143" s="2">
+        <f>ROUND([1]annualCYConc!$U102,0)</f>
+        <v>398</v>
+      </c>
+      <c r="C143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B144" s="2">
+        <f>ROUND([1]annualCYConc!$R79,0)</f>
+        <v>393</v>
+      </c>
+      <c r="C144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>2000</v>
+      </c>
+      <c r="B145" s="2">
+        <f>ROUND([1]annualCYConc!$R80,0)</f>
+        <v>405</v>
+      </c>
+      <c r="C145" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>2001</v>
+      </c>
+      <c r="B146" s="2">
+        <f>ROUND([1]annualCYConc!$R81,0)</f>
+        <v>395</v>
+      </c>
+      <c r="C146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>2002</v>
+      </c>
+      <c r="B147" s="2">
+        <f>ROUND([1]annualCYConc!$R82,0)</f>
+        <v>478</v>
+      </c>
+      <c r="C147" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>2003</v>
+      </c>
+      <c r="B148" s="2">
+        <f>ROUND([1]annualCYConc!$R83,0)</f>
+        <v>369</v>
+      </c>
+      <c r="C148" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>2004</v>
+      </c>
+      <c r="B149" s="2">
+        <f>ROUND([1]annualCYConc!$R84,0)</f>
+        <v>404</v>
+      </c>
+      <c r="C149" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>2005</v>
+      </c>
+      <c r="B150" s="2">
+        <f>ROUND([1]annualCYConc!$R85,0)</f>
+        <v>361</v>
+      </c>
+      <c r="C150" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>2006</v>
+      </c>
+      <c r="B151" s="2">
+        <f>ROUND([1]annualCYConc!$R86,0)</f>
+        <v>369</v>
+      </c>
+      <c r="C151" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>2007</v>
+      </c>
+      <c r="B152" s="2">
+        <f>ROUND([1]annualCYConc!$R87,0)</f>
+        <v>391</v>
+      </c>
+      <c r="C152" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>2008</v>
+      </c>
+      <c r="B153" s="2">
+        <f>ROUND([1]annualCYConc!$R88,0)</f>
+        <v>351</v>
+      </c>
+      <c r="C153" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>2009</v>
+      </c>
+      <c r="B154" s="2">
+        <f>ROUND([1]annualCYConc!$R89,0)</f>
+        <v>301</v>
+      </c>
+      <c r="C154" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>2010</v>
+      </c>
+      <c r="B155" s="2">
+        <f>ROUND([1]annualCYConc!$R90,0)</f>
+        <v>363</v>
+      </c>
+      <c r="C155" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>2011</v>
+      </c>
+      <c r="B156" s="2">
+        <f>ROUND([1]annualCYConc!$R91,0)</f>
+        <v>278</v>
+      </c>
+      <c r="C156" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>2012</v>
+      </c>
+      <c r="B157" s="2">
+        <f>ROUND([1]annualCYConc!$R92,0)</f>
+        <v>398</v>
+      </c>
+      <c r="C157" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>2013</v>
+      </c>
+      <c r="B158" s="2">
+        <f>ROUND([1]annualCYConc!$R93,0)</f>
+        <v>394</v>
+      </c>
+      <c r="C158" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>2014</v>
+      </c>
+      <c r="B159" s="2">
+        <f>ROUND([1]annualCYConc!$R94,0)</f>
+        <v>340</v>
+      </c>
+      <c r="C159" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>2015</v>
+      </c>
+      <c r="B160" s="2">
+        <f>ROUND([1]annualCYConc!$R95,0)</f>
+        <v>376</v>
+      </c>
+      <c r="C160" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>2016</v>
+      </c>
+      <c r="B161" s="2">
+        <f>ROUND([1]annualCYConc!$R96,0)</f>
+        <v>355</v>
+      </c>
+      <c r="C161" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>2017</v>
+      </c>
+      <c r="B162" s="2">
+        <f>ROUND([1]annualCYConc!$R97,0)</f>
+        <v>309</v>
+      </c>
+      <c r="C162" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>2018</v>
+      </c>
+      <c r="B163" s="2">
+        <f>ROUND([1]annualCYConc!$R98,0)</f>
+        <v>368</v>
+      </c>
+      <c r="C163" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>2019</v>
+      </c>
+      <c r="B164" s="2">
+        <f>ROUND([1]annualCYConc!$R99,0)</f>
+        <v>293</v>
+      </c>
+      <c r="C164" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>2020</v>
+      </c>
+      <c r="B165" s="2">
+        <f>ROUND([1]annualCYConc!$R100,0)</f>
+        <v>330</v>
+      </c>
+      <c r="C165" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>2021</v>
+      </c>
+      <c r="B166" s="2">
+        <f>ROUND([1]annualCYConc!$R101,0)</f>
+        <v>402</v>
+      </c>
+      <c r="C166" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>2022</v>
+      </c>
+      <c r="B167" s="2">
+        <f>ROUND([1]annualCYConc!$R102,0)</f>
+        <v>349</v>
+      </c>
+      <c r="C167" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B168" s="2">
+        <f>ROUND([1]annualCYConc!$J79,0)</f>
+        <v>496</v>
+      </c>
+      <c r="C168" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>2000</v>
+      </c>
+      <c r="B169" s="2">
+        <f>ROUND([1]annualCYConc!$J80,0)</f>
+        <v>557</v>
+      </c>
+      <c r="C169" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>2001</v>
+      </c>
+      <c r="B170" s="2">
+        <f>ROUND([1]annualCYConc!$J81,0)</f>
+        <v>622</v>
+      </c>
+      <c r="C170" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>2002</v>
+      </c>
+      <c r="B171" s="2">
+        <f>ROUND([1]annualCYConc!$J82,0)</f>
+        <v>852</v>
+      </c>
+      <c r="C171" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>2003</v>
+      </c>
+      <c r="B172" s="2">
+        <f>ROUND([1]annualCYConc!$J83,0)</f>
+        <v>611</v>
+      </c>
+      <c r="C172" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>2004</v>
+      </c>
+      <c r="B173" s="2">
+        <f>ROUND([1]annualCYConc!$J84,0)</f>
+        <v>655</v>
+      </c>
+      <c r="C173" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>2005</v>
+      </c>
+      <c r="B174" s="2">
+        <f>ROUND([1]annualCYConc!$J85,0)</f>
+        <v>416</v>
+      </c>
+      <c r="C174" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>2006</v>
+      </c>
+      <c r="B175" s="2">
+        <f>ROUND([1]annualCYConc!$J86,0)</f>
+        <v>487</v>
+      </c>
+      <c r="C175" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>2007</v>
+      </c>
+      <c r="B176" s="2">
+        <f>ROUND([1]annualCYConc!$J87,0)</f>
+        <v>533</v>
+      </c>
+      <c r="C176" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>2008</v>
+      </c>
+      <c r="B177" s="2">
+        <f>ROUND([1]annualCYConc!$J88,0)</f>
+        <v>384</v>
+      </c>
+      <c r="C177" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>2009</v>
+      </c>
+      <c r="B178" s="2">
+        <f>ROUND([1]annualCYConc!$J89,0)</f>
+        <v>426</v>
+      </c>
+      <c r="C178" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>2010</v>
+      </c>
+      <c r="B179" s="2">
+        <f>ROUND([1]annualCYConc!$J90,0)</f>
+        <v>512</v>
+      </c>
+      <c r="C179" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>2011</v>
+      </c>
+      <c r="B180" s="2">
+        <f>ROUND([1]annualCYConc!$J91,0)</f>
+        <v>346</v>
+      </c>
+      <c r="C180" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>2012</v>
+      </c>
+      <c r="B181" s="2">
+        <f>ROUND([1]annualCYConc!$J92,0)</f>
+        <v>722</v>
+      </c>
+      <c r="C181" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>2013</v>
+      </c>
+      <c r="B182" s="2">
+        <f>ROUND([1]annualCYConc!$J93,0)</f>
+        <v>644</v>
+      </c>
+      <c r="C182" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>2014</v>
+      </c>
+      <c r="B183" s="2">
+        <f>ROUND([1]annualCYConc!$J94,0)</f>
+        <v>427</v>
+      </c>
+      <c r="C183" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>2015</v>
+      </c>
+      <c r="B184" s="2">
+        <f>ROUND([1]annualCYConc!$J95,0)</f>
+        <v>458</v>
+      </c>
+      <c r="C184" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>2016</v>
+      </c>
+      <c r="B185" s="2">
+        <f>ROUND([1]annualCYConc!$J96,0)</f>
+        <v>465</v>
+      </c>
+      <c r="C185" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>2017</v>
+      </c>
+      <c r="B186" s="2">
+        <f>ROUND([1]annualCYConc!$J97,0)</f>
+        <v>432</v>
+      </c>
+      <c r="C186" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>2018</v>
+      </c>
+      <c r="B187" s="2">
+        <f>ROUND([1]annualCYConc!$J98,0)</f>
+        <v>687</v>
+      </c>
+      <c r="C187" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>2019</v>
+      </c>
+      <c r="B188" s="2">
+        <f>ROUND([1]annualCYConc!$J99,0)</f>
+        <v>381</v>
+      </c>
+      <c r="C188" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>2020</v>
+      </c>
+      <c r="B189" s="2">
+        <f>ROUND([1]annualCYConc!$J100,0)</f>
+        <v>605</v>
+      </c>
+      <c r="C189" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>2021</v>
+      </c>
+      <c r="B190" s="2">
+        <f>ROUND([1]annualCYConc!$J101,0)</f>
+        <v>713</v>
+      </c>
+      <c r="C190" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>2022</v>
+      </c>
+      <c r="B191" s="2">
+        <f>ROUND([1]annualCYConc!$J102,0)</f>
+        <v>602</v>
+      </c>
+      <c r="C191" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>